<commit_message>
Desarrollo del README del método de Bisección tema 2
</commit_message>
<xml_diff>
--- a/Tema_2/Métodos numéricos Raiz.xlsx
+++ b/Tema_2/Métodos numéricos Raiz.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prisc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prisc\Documents\Metodos_Numericos\Tema_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>x</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>Er(%)</t>
+  </si>
+  <si>
+    <t>Método de Punto Fijo</t>
+  </si>
+  <si>
+    <t>Método de la Secante</t>
   </si>
 </sst>
 </file>
@@ -177,7 +183,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -279,7 +285,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,19 +320,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -339,6 +333,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,22 +461,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -484,24 +478,18 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -511,25 +499,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -544,19 +523,40 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Cálculo" xfId="4" builtinId="22"/>
@@ -1831,253 +1831,253 @@
   <dimension ref="B2:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="B5:D6"/>
+      <selection activeCell="E2" sqref="E2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:12" ht="24.95" customHeight="1">
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="F4" s="8"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="2:12">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="20"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="2:12">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>0</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:12">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="18" t="s">
+      <c r="K8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="18" t="s">
+      <c r="L8" s="16" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:12">
-      <c r="B9" s="15">
+      <c r="B9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="14">
         <f>C6</f>
         <v>0</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="14">
         <f>D6</f>
         <v>1</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="14">
         <f>(C9+D9)/2</f>
         <v>0.5</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="14">
         <f t="shared" ref="F9:H12" si="0">(C9)^3-4*(C9)+1</f>
         <v>1</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="14">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="14">
         <f t="shared" si="0"/>
         <v>-0.875</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="14">
         <f>F9*H9</f>
         <v>-0.875</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="14">
         <f>G9*H9</f>
         <v>1.75</v>
       </c>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="11">
+      <c r="B10" s="9">
         <v>2</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="10">
         <f>IF(I9&lt;0,C9,E9)</f>
         <v>0</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="10">
         <f>IF(J9&lt;0,D9,E9)</f>
         <v>0.5</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <f>(C10*G10-D10*F10)/(G10-F10)</f>
         <v>0.26666666666666666</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="10">
         <f t="shared" si="0"/>
         <v>-0.875</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="10">
         <f t="shared" si="0"/>
         <v>-4.7703703703703582E-2</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="10">
         <f>F10*H10</f>
         <v>-4.7703703703703582E-2</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="10">
         <f>G10*H10</f>
         <v>4.1740740740740634E-2</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="10">
         <f>ABS(E9-E10)</f>
         <v>0.23333333333333334</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="11">
         <f>K10/E9</f>
         <v>0.46666666666666667</v>
       </c>
     </row>
     <row r="11" spans="2:12">
-      <c r="B11" s="11">
+      <c r="B11" s="9">
         <v>3</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="10">
         <f>IF(I10&lt;0,C10,E10)</f>
         <v>0</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="10">
         <f>IF(J10&lt;0,D10,E10)</f>
         <v>0.26666666666666666</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="10">
         <f>(C11*G11-D11*F11)/(G11-F11)</f>
         <v>0.25452488687782809</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="10">
         <f t="shared" si="0"/>
         <v>-4.7703703703703582E-2</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="10">
         <f t="shared" si="0"/>
         <v>-1.6106826255222195E-3</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="10">
         <f>F11*H11</f>
         <v>-1.6106826255222195E-3</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="10">
         <f>G11*H11</f>
         <v>7.6835526728615306E-5</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="10">
         <f>ABS(E10-E11)</f>
         <v>1.2141779788838569E-2</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="11">
         <f>K11/E10</f>
         <v>4.5531674208144635E-2</v>
       </c>
     </row>
     <row r="12" spans="2:12">
-      <c r="B12" s="11">
+      <c r="B12" s="9">
         <v>4</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="10">
         <f>IF(I11&lt;0,C11,E11)</f>
         <v>0</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="10">
         <f>IF(J11&lt;0,D11,E11)</f>
         <v>0.25452488687782809</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="10">
         <f>(C12*G12-D12*F12)/(G12-F12)</f>
         <v>0.25411558731646311</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="10">
         <f t="shared" si="0"/>
         <v>-1.6106826255222195E-3</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="10">
         <f t="shared" si="0"/>
         <v>-5.290338973540365E-5</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="10">
         <f>F12*H12</f>
         <v>-5.290338973540365E-5</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="10">
         <f>G12*H12</f>
         <v>8.5210570678045186E-8</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="10">
         <f>ABS(E11-E12)</f>
         <v>4.0929956136498413E-4</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="11">
         <f>K12/E11</f>
         <v>1.6080924988739818E-3</v>
       </c>
@@ -2139,241 +2139,250 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:K12"/>
+  <dimension ref="B2:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="E2" sqref="E2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
+    <row r="2" spans="2:11" ht="23.25" customHeight="1">
+      <c r="E2" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+    </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="20"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="18">
         <v>0</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="19" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="16">
+      <c r="B9" s="14">
         <f>C6</f>
         <v>0</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="14">
         <f>D6</f>
         <v>1</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D9" s="14">
         <f t="shared" ref="D9:E12" si="0">(B9)^3-4*(B9)+1</f>
         <v>1</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="14">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="14">
         <f>(B9*E9-C9*D9)/(E9-D9)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="14">
         <f>(F9)^3-4*(F9)+1</f>
         <v>-0.29629629629629628</v>
       </c>
-      <c r="H9" s="16">
+      <c r="H9" s="14">
         <f>D9*G9</f>
         <v>-0.29629629629629628</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="14">
         <f>E9*G9</f>
         <v>0.59259259259259256</v>
       </c>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" s="12">
+      <c r="B10" s="10">
         <f>IF(H9&lt;0,B9,F9)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="10">
         <f>IF(I9&lt;0,C9,F9)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <f t="shared" si="0"/>
         <v>-0.29629629629629628</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="10">
         <f>(B10*E10-C10*D10)/(E10-D10)</f>
         <v>0.25714285714285712</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="10">
         <f>(F10)^3-4*(F10)+1</f>
         <v>-1.156851311953333E-2</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="10">
         <f>D10*G10</f>
         <v>-1.156851311953333E-2</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="10">
         <f>E10*G10</f>
         <v>3.4277075909728383E-3</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="10">
         <f>ABS(F9-F10)</f>
         <v>7.6190476190476197E-2</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="11">
         <f>J10/F10</f>
         <v>0.29629629629629634</v>
       </c>
     </row>
     <row r="11" spans="2:11">
-      <c r="B11" s="12">
+      <c r="B11" s="10">
         <f>IF(H10&lt;0,B10,F10)</f>
         <v>0</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="10">
         <f>IF(I10&lt;0,C10,F10)</f>
         <v>0.25714285714285712</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="10">
         <f t="shared" si="0"/>
         <v>-1.156851311953333E-2</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="10">
         <f>(B11*E11-C11*D11)/(E11-D11)</f>
         <v>0.25420211662170578</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="10">
         <f>(F11)^3-4*(F11)+1</f>
         <v>-3.82252082108403E-4</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="10">
         <f>D11*G11</f>
         <v>-3.82252082108403E-4</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="10">
         <f>E11*G11</f>
         <v>4.4220882268399922E-6</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="10">
         <f t="shared" ref="J11:J12" si="1">ABS(F10-F11)</f>
         <v>2.9407405211513415E-3</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="11">
         <f>J11/F11</f>
         <v>1.1568513119533316E-2</v>
       </c>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="12">
+      <c r="B12" s="10">
         <f>IF(H11&lt;0,B11,F11)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="10">
         <f>IF(I11&lt;0,C11,F11)</f>
         <v>0.25420211662170578</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="10">
         <f t="shared" si="0"/>
         <v>-3.82252082108403E-4</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="10">
         <f>(B12*E12-C12*D12)/(E12-D12)</f>
         <v>0.25410498446232094</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="10">
         <f>(F12)^3-4*(F12)+1</f>
         <v>-1.2545916849404648E-5</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="10">
         <f>D12*G12</f>
         <v>-1.2545916849404648E-5</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="10">
         <f>E12*G12</f>
         <v>4.7957028376438225E-9</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="10">
         <f t="shared" si="1"/>
         <v>9.7132159384838435E-5</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="11">
         <f t="shared" ref="K12" si="2">J12/F12</f>
         <v>3.8225208210837492E-4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2384,7 +2393,7 @@
   <dimension ref="B1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="B5:C8"/>
+      <selection activeCell="E2" sqref="E2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2401,206 +2410,206 @@
       <c r="I1" s="5"/>
     </row>
     <row r="2" spans="2:13" ht="24.95" customHeight="1">
-      <c r="D2" s="7"/>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="2:13">
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="2:13">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="14" t="s">
+      <c r="C4" s="39"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="K4" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:13">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="33">
         <v>3.5</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="30">
+      <c r="D5" s="21"/>
+      <c r="E5" s="24">
         <v>1</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="25">
         <f>C5</f>
         <v>3.5</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="25">
         <f>(F5^3-27)</f>
         <v>15.875</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="25">
         <f>(3*F5^2)</f>
         <v>36.75</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="25">
         <f>(F5-(G5/H5))</f>
         <v>3.0680272108843538</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="25">
         <f>ABS(F5-I5)</f>
         <v>0.43197278911564618</v>
       </c>
-      <c r="K5" s="36">
+      <c r="K5" s="29">
         <f>J5/I5</f>
         <v>0.1407982261640798</v>
       </c>
-      <c r="L5" s="30" t="str">
+      <c r="L5" s="24" t="str">
         <f>IF(J5&gt;C8,"Continua",I5)</f>
         <v>Continua</v>
       </c>
     </row>
     <row r="6" spans="2:13">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="30">
+      <c r="D6" s="21"/>
+      <c r="E6" s="24">
         <v>2</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="25">
         <f>I5</f>
         <v>3.0680272108843538</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="25">
         <f t="shared" ref="G6:G10" si="0">(F6^3-27)</f>
         <v>1.8786988162843485</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="25">
         <f t="shared" ref="H6:H10" si="1">(3*F6^2)</f>
         <v>28.238372900180483</v>
       </c>
-      <c r="I6" s="31">
-        <f t="shared" ref="I6:I8" si="2">(F6-(G6/H6))</f>
+      <c r="I6" s="25">
+        <f t="shared" ref="I6" si="2">(F6-(G6/H6))</f>
         <v>3.001497215585923</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="25">
         <f t="shared" ref="J6:J10" si="3">ABS(F6-I6)</f>
         <v>6.6529995298430844E-2</v>
       </c>
-      <c r="K6" s="36">
+      <c r="K6" s="29">
         <f t="shared" ref="K6:K10" si="4">J6/I6</f>
         <v>2.2165602870780444E-2</v>
       </c>
-      <c r="L6" s="30" t="str">
+      <c r="L6" s="24" t="str">
         <f>IF(J6&gt;C8,"Continua",I6)</f>
         <v>Continua</v>
       </c>
     </row>
     <row r="7" spans="2:13">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="30">
+      <c r="D7" s="21"/>
+      <c r="E7" s="24">
         <v>3</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="25">
         <f>I6</f>
         <v>3.001497215585923</v>
       </c>
-      <c r="G7" s="31">
+      <c r="G7" s="25">
         <f t="shared" si="0"/>
         <v>4.0444999066753695E-2</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="25">
         <f t="shared" si="1"/>
         <v>27.026956605510144</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="25">
         <f t="shared" ref="I7:I10" si="5">(F7-(G7/H7))</f>
         <v>3.0000007467212595</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="25">
         <f t="shared" si="3"/>
         <v>1.4964688646634805E-3</v>
       </c>
-      <c r="K7" s="36">
+      <c r="K7" s="29">
         <f t="shared" si="4"/>
         <v>4.9882283072728937E-4</v>
       </c>
-      <c r="L7" s="30" t="str">
+      <c r="L7" s="24" t="str">
         <f>IF(J7&gt;C9,"Continua",I7)</f>
         <v>Continua</v>
       </c>
     </row>
     <row r="8" spans="2:13">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="33">
         <v>1E-3</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="30">
+      <c r="D8" s="21"/>
+      <c r="E8" s="24">
         <v>4</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="25">
         <f>I7</f>
         <v>3.0000007467212595</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="25">
         <f t="shared" si="0"/>
         <v>2.0161479021396644E-5</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="25">
         <f t="shared" si="1"/>
         <v>27.00001344098434</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="25">
         <f t="shared" si="5"/>
         <v>3.0000000000001861</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="25">
         <f t="shared" si="3"/>
         <v>7.4672107341910987E-7</v>
       </c>
-      <c r="K8" s="36">
+      <c r="K8" s="29">
         <f t="shared" si="4"/>
         <v>2.4890702447302118E-7</v>
       </c>
-      <c r="L8" s="30" t="str">
+      <c r="L8" s="24" t="str">
         <f>IF(J8&gt;C10,"Continua",I8)</f>
         <v>Continua</v>
       </c>
@@ -2608,100 +2617,100 @@
     <row r="9" spans="2:13">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="E9" s="30">
+      <c r="E9" s="24">
         <v>5</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="25">
         <f>I8</f>
         <v>3.0000000000001861</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="25">
         <f t="shared" si="0"/>
         <v>5.0199844281451078E-12</v>
       </c>
-      <c r="H9" s="31">
+      <c r="H9" s="25">
         <f t="shared" si="1"/>
         <v>27.000000000003347</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="25">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="25">
         <f t="shared" si="3"/>
         <v>1.8607337892717624E-13</v>
       </c>
-      <c r="K9" s="36">
+      <c r="K9" s="29">
         <f t="shared" si="4"/>
         <v>6.2024459642392075E-14</v>
       </c>
-      <c r="L9" s="30" t="str">
+      <c r="L9" s="24" t="str">
         <f>IF(J9&gt;C11,"Continua",I9)</f>
         <v>Continua</v>
       </c>
     </row>
     <row r="10" spans="2:13">
-      <c r="E10" s="30">
+      <c r="E10" s="24">
         <v>6</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="25">
         <f>I9</f>
         <v>3</v>
       </c>
-      <c r="G10" s="31">
+      <c r="G10" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="31">
+      <c r="H10" s="25">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="25">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K10" s="36">
+      <c r="K10" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L10" s="31">
+      <c r="L10" s="25">
         <f>IF(J10&gt;C12,"Continua",I10)</f>
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:13">
-      <c r="E11" s="24"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="29"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="23"/>
     </row>
     <row r="12" spans="2:13">
-      <c r="E12" s="24"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="29"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="23"/>
     </row>
     <row r="13" spans="2:13">
-      <c r="E13" s="24"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="29"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="23"/>
     </row>
     <row r="14" spans="2:13">
       <c r="F14" s="2"/>
@@ -2760,155 +2769,164 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:K9"/>
+  <dimension ref="B2:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="B5:D8"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
+    <row r="2" spans="2:11" ht="30" customHeight="1">
+      <c r="E2" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+    </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="18" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="16" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="15">
+      <c r="D5" s="35"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="13">
         <v>1</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="13">
         <f>C7</f>
         <v>0</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="27">
         <f>C8</f>
         <v>0</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="14">
         <f>(H5^3+1)/4</f>
         <v>0.25</v>
       </c>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="11">
+      <c r="D6" s="35"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="9">
         <v>2</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <f>H5+1</f>
         <v>1</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="10">
         <f>I5</f>
         <v>0.25</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="10">
         <f t="shared" ref="I6:I7" si="0">(H6^3+1)/4</f>
         <v>0.25390625</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="10">
         <f>ABS(I6-H6)</f>
         <v>3.90625E-3</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="11">
         <f>J6/I6</f>
         <v>1.5384615384615385E-2</v>
       </c>
     </row>
     <row r="7" spans="2:11">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="35">
         <v>0</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="11">
+      <c r="D7" s="35"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="9">
         <v>3</v>
       </c>
-      <c r="G7" s="11">
-        <f t="shared" ref="G7" si="1">G6+1</f>
+      <c r="G7" s="9">
+        <f t="shared" ref="G7:G21" si="1">G6+1</f>
         <v>2</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="10">
         <f t="shared" ref="H7" si="2">I6</f>
         <v>0.25390625</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="10">
         <f t="shared" si="0"/>
         <v>0.25409223139286041</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="10">
         <f t="shared" ref="J7" si="3">ABS(I6-I7)</f>
         <v>1.859813928604126E-4</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="11">
         <f>J7/I7</f>
         <v>7.3194442758409486E-4</v>
       </c>
     </row>
     <row r="8" spans="2:11">
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="35">
         <v>0</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="2:11">
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="E2:H2"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -2921,308 +2939,318 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:G18"/>
+  <dimension ref="B2:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
+    <row r="2" spans="2:7">
+      <c r="C2" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+    </row>
     <row r="4" spans="2:7" ht="18">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="39"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="21"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="41" t="s">
+      <c r="F8" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="42" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="42">
+      <c r="B9" s="43">
         <v>1</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="43">
         <v>2</v>
       </c>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="42">
+      <c r="B10" s="43">
         <v>2</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="43">
         <v>5</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="43">
         <f>EXP(-C10)-C10</f>
         <v>-4.9932620530009144</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="43">
         <f>EXP(-C9)-C9</f>
         <v>-1.8646647167633872</v>
       </c>
-      <c r="F10" s="42">
+      <c r="F10" s="43">
         <f>C10-C9</f>
         <v>3</v>
       </c>
-      <c r="G10" s="42"/>
+      <c r="G10" s="43"/>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="42">
+      <c r="B11" s="43">
         <v>3</v>
       </c>
-      <c r="C11" s="42">
+      <c r="C11" s="43">
         <f>C10-(D10*F10)/(D10-E10)</f>
         <v>0.21198014666293297</v>
       </c>
-      <c r="D11" s="42">
+      <c r="D11" s="43">
         <f>EXP(-C11)-C11</f>
         <v>0.59700061171181273</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="43">
         <f>EXP(-C10)-C10</f>
         <v>-4.9932620530009144</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="43">
         <f>C11-C10</f>
         <v>-4.788019853337067</v>
       </c>
-      <c r="G11" s="43">
+      <c r="G11" s="44">
         <f>ABS((C11-C10)/C11)</f>
         <v>22.587114542148321</v>
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="42">
+      <c r="B12" s="43">
         <v>4</v>
       </c>
-      <c r="C12" s="42">
+      <c r="C12" s="43">
         <f t="shared" ref="C12:C18" si="0">C11-(D11*F11)/(D11-E11)</f>
         <v>0.72330688616908523</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="43">
         <f t="shared" ref="D12:D18" si="1">EXP(-C12)-C12</f>
         <v>-0.23816160600467956</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="43">
         <f t="shared" ref="E12:E18" si="2">EXP(-C11)-C11</f>
         <v>0.59700061171181273</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="43">
         <f t="shared" ref="F12:F18" si="3">C12-C11</f>
         <v>0.51132673950615226</v>
       </c>
-      <c r="G12" s="43">
+      <c r="G12" s="44">
         <f t="shared" ref="G12:G18" si="4">ABS((C12-C11)/C12)</f>
         <v>0.70692917388680987</v>
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="42">
+      <c r="B13" s="43">
         <v>5</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="43">
         <f t="shared" si="0"/>
         <v>0.57749282167884863</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="43">
         <f t="shared" si="1"/>
         <v>-1.6188928850512374E-2</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="43">
         <f t="shared" si="2"/>
         <v>-0.23816160600467956</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F13" s="43">
         <f t="shared" si="3"/>
         <v>-0.14581406449023659</v>
       </c>
-      <c r="G13" s="43">
+      <c r="G13" s="44">
         <f t="shared" si="4"/>
         <v>0.25249502507465921</v>
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="42">
+      <c r="B14" s="43">
         <v>6</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="43">
         <f t="shared" si="0"/>
         <v>0.56685829879206573</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="43">
         <f t="shared" si="1"/>
         <v>4.4664573547015252E-4</v>
       </c>
-      <c r="E14" s="42">
+      <c r="E14" s="43">
         <f t="shared" si="2"/>
         <v>-1.6188928850512374E-2</v>
       </c>
-      <c r="F14" s="42">
+      <c r="F14" s="43">
         <f t="shared" si="3"/>
         <v>-1.0634522886782904E-2</v>
       </c>
-      <c r="G14" s="43">
+      <c r="G14" s="44">
         <f t="shared" si="4"/>
         <v>1.8760460787897625E-2</v>
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="42">
+      <c r="B15" s="43">
         <v>7</v>
       </c>
-      <c r="C15" s="42">
+      <c r="C15" s="43">
         <f t="shared" si="0"/>
         <v>0.56714382330290192</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="43">
         <f t="shared" si="1"/>
         <v>-8.3511979387385082E-7</v>
       </c>
-      <c r="E15" s="42">
+      <c r="E15" s="43">
         <f t="shared" si="2"/>
         <v>4.4664573547015252E-4</v>
       </c>
-      <c r="F15" s="42">
+      <c r="F15" s="43">
         <f t="shared" si="3"/>
         <v>2.8552451083618813E-4</v>
       </c>
-      <c r="G15" s="43">
+      <c r="G15" s="44">
         <f t="shared" si="4"/>
         <v>5.0344286423391815E-4</v>
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="42">
+      <c r="B16" s="43">
         <v>8</v>
       </c>
-      <c r="C16" s="42">
+      <c r="C16" s="43">
         <f t="shared" si="0"/>
         <v>0.56714329043726575</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="43">
         <f t="shared" si="1"/>
         <v>-4.3067993615863998E-11</v>
       </c>
-      <c r="E16" s="42">
+      <c r="E16" s="43">
         <f t="shared" si="2"/>
         <v>-8.3511979387385082E-7</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F16" s="43">
         <f t="shared" si="3"/>
         <v>-5.3286563617138683E-7</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="44">
         <f t="shared" si="4"/>
         <v>9.3956085729331127E-7</v>
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="42">
+      <c r="B17" s="43">
         <v>9</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="43">
         <f t="shared" si="0"/>
         <v>0.56714329040978384</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E17" s="42">
+      <c r="E17" s="43">
         <f t="shared" si="2"/>
         <v>-4.3067993615863998E-11</v>
       </c>
-      <c r="F17" s="42">
+      <c r="F17" s="43">
         <f t="shared" si="3"/>
         <v>-2.7481905640058812E-11</v>
       </c>
-      <c r="G17" s="43">
+      <c r="G17" s="44">
         <f t="shared" si="4"/>
         <v>4.8456723556055877E-11</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="42">
+      <c r="B18" s="43">
         <v>10</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="43">
         <f t="shared" si="0"/>
         <v>0.56714329040978384</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="43">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E18" s="42">
+      <c r="E18" s="43">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F18" s="42">
+      <c r="F18" s="43">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G18" s="43">
+      <c r="G18" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>